<commit_message>
Removed the existing cell displaying the current date (it was not updated automatically)
</commit_message>
<xml_diff>
--- a/OutilDevis/DevisVierge.xlsx
+++ b/OutilDevis/DevisVierge.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Rénovation bâtiments anciens</t>
   </si>
   <si>
     <t xml:space="preserve">Maçonnerie terre crue : pisé, torchis, adobes, …</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devis n° ?????????????, édité le 12/01/20, valable 30 jours</t>
   </si>
   <si>
     <t xml:space="preserve">Entrer ici les coordonnées du client</t>
@@ -329,9 +326,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>696600</xdr:colOff>
+      <xdr:colOff>696240</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -344,8 +341,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4686120" y="28800"/>
-          <a:ext cx="1101240" cy="738000"/>
+          <a:off x="4690080" y="28800"/>
+          <a:ext cx="1100520" cy="737640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -366,9 +363,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>378720</xdr:colOff>
+      <xdr:colOff>378360</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -383,8 +380,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2167920" y="28800"/>
-          <a:ext cx="1870200" cy="925920"/>
+          <a:off x="2170440" y="28800"/>
+          <a:ext cx="1870920" cy="925560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -405,9 +402,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>186480</xdr:colOff>
+      <xdr:colOff>186120</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -421,7 +418,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="28080"/>
-          <a:ext cx="1821960" cy="370440"/>
+          <a:ext cx="1824120" cy="370080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -443,11 +440,11 @@
   </sheetPr>
   <dimension ref="A7:G58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.69"/>
@@ -477,9 +474,7 @@
       <c r="G8" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -498,7 +493,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -521,24 +516,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,7 +886,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="9" t="n">
@@ -901,7 +896,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="9" t="n">
@@ -911,7 +906,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="9" t="n">
@@ -921,7 +916,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -932,7 +927,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -943,7 +938,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -954,21 +949,21 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>

</xml_diff>